<commit_message>
added one-hot-encoding to classification.py
</commit_message>
<xml_diff>
--- a/supplements/FACTORIZATION_TABLE.xlsx
+++ b/supplements/FACTORIZATION_TABLE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800EE883-46FC-48B7-8E1D-509DC7987397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A65F9-AE5D-4AB6-A0A0-A38A946D5B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>feature</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>7TH DAY ADVENTIST</t>
+  </si>
+  <si>
+    <t>dbsource</t>
+  </si>
+  <si>
+    <t>carevue</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>metavision</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,35 +1161,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1185,10 +1197,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,10 +1208,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,65 +1219,65 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1273,10 +1285,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1284,43 +1296,43 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1328,7 +1340,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2">
         <v>-1</v>
@@ -1339,10 +1351,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1350,10 +1362,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1361,10 +1373,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1372,18 +1384,18 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
@@ -1391,24 +1403,24 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1416,7 +1428,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -1427,10 +1439,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1438,10 +1450,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1449,10 +1461,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1460,10 +1472,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1471,10 +1483,10 @@
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C34" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1482,10 +1494,10 @@
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C35" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1493,10 +1505,10 @@
         <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1504,10 +1516,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1515,10 +1527,10 @@
         <v>31</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C38" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1526,10 +1538,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1537,10 +1549,10 @@
         <v>31</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C40" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1548,10 +1560,10 @@
         <v>31</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C41" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1559,10 +1571,10 @@
         <v>31</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C42" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1570,42 +1582,75 @@
         <v>31</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C43" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C44" s="2">
-        <v>-1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C45" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C49" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added kPrototypes clustering, exported plots for text first draft, cleanup
</commit_message>
<xml_diff>
--- a/supplements/FACTORIZATION_TABLE.xlsx
+++ b/supplements/FACTORIZATION_TABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4A65F9-AE5D-4AB6-A0A0-A38A946D5B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93CE79-D8AE-4881-A490-48B564FCADA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added Data Upload Page
</commit_message>
<xml_diff>
--- a/supplements/FACTORIZATION_TABLE.xlsx
+++ b/supplements/FACTORIZATION_TABLE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\MA_thesis\supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93CE79-D8AE-4881-A490-48B564FCADA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436798F2-9286-4290-A373-881099BF9DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1629,7 +1629,7 @@
         <v>48</v>
       </c>
       <c r="C47" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1640,7 +1640,7 @@
         <v>49</v>
       </c>
       <c r="C48" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1651,7 +1651,7 @@
         <v>50</v>
       </c>
       <c r="C49" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>